<commit_message>
Task 2.3: Triples for external and internal URIs
</commit_message>
<xml_diff>
--- a/Task 2.3/zip_code_ranges.xlsx
+++ b/Task 2.3/zip_code_ranges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronaltrock/PycharmProjects/Pizza_KG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43A5BC7B-C8CA-074D-A85E-1BB20E3C28FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A91A67-53D4-9E47-8D2D-780F05EB22A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{727DFE31-8A58-B04B-83EE-A261BE9662FB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
   <si>
     <t>ID</t>
   </si>
@@ -69,9 +69,6 @@
     <t>AR</t>
   </si>
   <si>
-    <t>Arkansas (Texarkana)</t>
-  </si>
-  <si>
     <t>Arizona</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>CT</t>
   </si>
   <si>
-    <t>Dist of Columbia</t>
-  </si>
-  <si>
     <t>DC</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>GA</t>
   </si>
   <si>
-    <t>Georga (Atlanta)</t>
-  </si>
-  <si>
     <t>Hawaii</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>IA</t>
   </si>
   <si>
-    <t>Iowa (OMAHA)</t>
-  </si>
-  <si>
     <t>Idaho</t>
   </si>
   <si>
@@ -177,9 +165,6 @@
     <t>MA</t>
   </si>
   <si>
-    <t>Massachusetts (Andover)</t>
-  </si>
-  <si>
     <t>Maryland</t>
   </si>
   <si>
@@ -204,9 +189,6 @@
     <t>MN</t>
   </si>
   <si>
-    <t>kc96 DataMO</t>
-  </si>
-  <si>
     <t>MO</t>
   </si>
   <si>
@@ -216,9 +198,6 @@
     <t>MS</t>
   </si>
   <si>
-    <t>Mississippi(Warren)</t>
-  </si>
-  <si>
     <t>Montana</t>
   </si>
   <si>
@@ -267,15 +246,9 @@
     <t>NV</t>
   </si>
   <si>
-    <t>New York (Fishers Is)</t>
-  </si>
-  <si>
     <t>NY</t>
   </si>
   <si>
-    <t>New York</t>
-  </si>
-  <si>
     <t>Ohio</t>
   </si>
   <si>
@@ -330,18 +303,12 @@
     <t>TN</t>
   </si>
   <si>
-    <t>Texas (Austin)</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
     <t>Texas</t>
   </si>
   <si>
-    <t>Texas (El Paso)</t>
-  </si>
-  <si>
     <t>Utah</t>
   </si>
   <si>
@@ -382,6 +349,15 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>New York State</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
   </si>
 </sst>
 </file>
@@ -762,10 +738,13 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -840,7 +819,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -857,10 +836,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="2">
         <v>85001</v>
@@ -874,10 +853,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D7" s="2">
         <v>90001</v>
@@ -891,10 +870,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D8" s="2">
         <v>80001</v>
@@ -908,10 +887,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="2">
         <v>6001</v>
@@ -925,10 +904,10 @@
         <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D10" s="2">
         <v>6401</v>
@@ -942,10 +921,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2">
         <v>20001</v>
@@ -959,10 +938,10 @@
         <v>74</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="2">
         <v>20042</v>
@@ -976,10 +955,10 @@
         <v>63</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2">
         <v>20799</v>
@@ -993,10 +972,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2">
         <v>19701</v>
@@ -1010,10 +989,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2">
         <v>32004</v>
@@ -1027,10 +1006,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2">
         <v>30001</v>
@@ -1044,10 +1023,10 @@
         <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="2">
         <v>39901</v>
@@ -1061,10 +1040,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2">
         <v>96701</v>
@@ -1078,10 +1057,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2">
         <v>50001</v>
@@ -1095,10 +1074,10 @@
         <v>66</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D20" s="2">
         <v>68119</v>
@@ -1112,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>0</v>
@@ -1129,10 +1108,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D22" s="2">
         <v>60001</v>
@@ -1146,10 +1125,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D23" s="2">
         <v>46001</v>
@@ -1163,10 +1142,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D24" s="2">
         <v>66002</v>
@@ -1180,10 +1159,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2">
         <v>40003</v>
@@ -1197,10 +1176,10 @@
         <v>68</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2">
         <v>70001</v>
@@ -1214,10 +1193,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2">
         <v>71234</v>
@@ -1231,10 +1210,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2">
         <v>1001</v>
@@ -1248,10 +1227,10 @@
         <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D29" s="2">
         <v>5501</v>
@@ -1265,10 +1244,10 @@
         <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D30" s="2">
         <v>20331</v>
@@ -1282,10 +1261,10 @@
         <v>78</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D31" s="2">
         <v>20335</v>
@@ -1299,10 +1278,10 @@
         <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D32" s="2">
         <v>20812</v>
@@ -1316,10 +1295,10 @@
         <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D33" s="2">
         <v>3901</v>
@@ -1333,10 +1312,10 @@
         <v>27</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D34" s="2">
         <v>48001</v>
@@ -1350,10 +1329,10 @@
         <v>28</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D35" s="2">
         <v>55001</v>
@@ -1367,10 +1346,10 @@
         <v>57</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D36" s="2">
         <v>63001</v>
@@ -1384,10 +1363,10 @@
         <v>29</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D37" s="2">
         <v>38601</v>
@@ -1401,10 +1380,10 @@
         <v>59</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D38" s="2">
         <v>71233</v>
@@ -1418,10 +1397,10 @@
         <v>31</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D39" s="2">
         <v>59001</v>
@@ -1435,10 +1414,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D40" s="2">
         <v>27006</v>
@@ -1452,10 +1431,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D41" s="2">
         <v>58001</v>
@@ -1469,10 +1448,10 @@
         <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D42" s="2">
         <v>68001</v>
@@ -1486,10 +1465,10 @@
         <v>32</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D43" s="2">
         <v>68122</v>
@@ -1503,10 +1482,10 @@
         <v>34</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D44" s="2">
         <v>3031</v>
@@ -1520,10 +1499,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D45" s="2">
         <v>7001</v>
@@ -1537,10 +1516,10 @@
         <v>36</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D46" s="2">
         <v>87001</v>
@@ -1554,10 +1533,10 @@
         <v>33</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D47" s="2">
         <v>88901</v>
@@ -1571,10 +1550,10 @@
         <v>60</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D48" s="2">
         <v>6390</v>
@@ -1588,10 +1567,10 @@
         <v>37</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D49" s="2">
         <v>10001</v>
@@ -1605,10 +1584,10 @@
         <v>40</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D50" s="2">
         <v>43001</v>
@@ -1622,10 +1601,10 @@
         <v>70</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D51" s="2">
         <v>73001</v>
@@ -1639,10 +1618,10 @@
         <v>41</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D52" s="2">
         <v>73401</v>
@@ -1656,10 +1635,10 @@
         <v>42</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D53" s="2">
         <v>97001</v>
@@ -1673,10 +1652,10 @@
         <v>43</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D54" s="2">
         <v>15001</v>
@@ -1690,10 +1669,10 @@
         <v>44</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D55" s="2">
         <v>0</v>
@@ -1707,10 +1686,10 @@
         <v>45</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D56" s="2">
         <v>2801</v>
@@ -1724,10 +1703,10 @@
         <v>46</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D57" s="2">
         <v>29001</v>
@@ -1741,10 +1720,10 @@
         <v>47</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D58" s="2">
         <v>57001</v>
@@ -1758,10 +1737,10 @@
         <v>48</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D59" s="2">
         <v>37010</v>
@@ -1775,10 +1754,10 @@
         <v>49</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D60" s="2">
         <v>73301</v>
@@ -1792,10 +1771,10 @@
         <v>71</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D61" s="2">
         <v>75001</v>
@@ -1809,10 +1788,10 @@
         <v>72</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D62" s="2">
         <v>75503</v>
@@ -1826,10 +1805,10 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D63" s="2">
         <v>88510</v>
@@ -1843,10 +1822,10 @@
         <v>50</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D64" s="2">
         <v>84001</v>
@@ -1860,10 +1839,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D65" s="2">
         <v>20040</v>
@@ -1877,10 +1856,10 @@
         <v>75</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D66" s="2">
         <v>20040</v>
@@ -1894,10 +1873,10 @@
         <v>76</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D67" s="2">
         <v>20042</v>
@@ -1911,10 +1890,10 @@
         <v>52</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D68" s="2">
         <v>22001</v>
@@ -1928,10 +1907,10 @@
         <v>51</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D69" s="2">
         <v>5001</v>
@@ -1945,10 +1924,10 @@
         <v>62</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D70" s="2">
         <v>5601</v>
@@ -1962,10 +1941,10 @@
         <v>53</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D71" s="2">
         <v>98001</v>
@@ -1979,10 +1958,10 @@
         <v>55</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D72" s="2">
         <v>53001</v>
@@ -1996,10 +1975,10 @@
         <v>54</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D73" s="2">
         <v>24701</v>
@@ -2013,10 +1992,10 @@
         <v>56</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D74" s="2">
         <v>82001</v>

</xml_diff>